<commit_message>
attack_data_sources field in MD and XLSX to YAML scripts
python scripts md_to_yaml.py and xlsx_to_md.py were modified. I added the attack_data_sources metadata field.

To separate more than one data sources, use a comma(,)
</commit_message>
<xml_diff>
--- a/resources/scripts/templates/xlsx_to_yaml_template.xlsx
+++ b/resources/scripts/templates/xlsx_to_yaml_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6584cd57bed31e5/Cyb3rPandaH/Open Threat Research/OSSEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyb3rpandah/Documents/GitHub/OSSEM/resources/scripts/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{039A492C-0ADB-F648-BD96-AD6C70E06611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1006D53E-2844-7E4C-8331-27803E1EA2E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721138BD-F653-2442-8A88-E45AC3097EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC128728-4C07-5149-9741-AEC38C8FC335}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>title</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>version test</t>
+  </si>
+  <si>
+    <t>attack_data_sources</t>
+  </si>
+  <si>
+    <t>ATT&amp;CK_datasource_1,ATT&amp;CK_datasource_2</t>
   </si>
 </sst>
 </file>
@@ -340,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -648,11 +654,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -685,6 +717,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,16 +1033,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5A1C5E-2AE3-9946-9B05-27E906269621}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1055,283 +1089,291 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="21" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-    </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="21" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D9" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E9" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B10" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E20" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D21" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
     <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="3"/>
-    </row>
     <row r="26" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>